<commit_message>
Fix E2E tests and ingestion logic
Fixed excelUtils.ts to handle empty rows correctly. Restored DataLoaderPage.tsx content. Added error logging to ingestionCoordinator.ts. Updated E2E test assertions to match generated fixtures. Cleaned up debug logs.
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/EquipmentList_TEST.xlsx
+++ b/tests/fixtures/excel/EquipmentList_TEST.xlsx
@@ -397,82 +397,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Area</v>
+        <v>TOOL</v>
       </c>
       <c r="B1" t="str">
-        <v>Line</v>
+        <v>TYPE</v>
       </c>
       <c r="C1" t="str">
-        <v>Station</v>
+        <v>AREA</v>
       </c>
       <c r="D1" t="str">
-        <v>Robot Name</v>
+        <v>STATION</v>
       </c>
       <c r="E1" t="str">
-        <v>Robot Model</v>
+        <v>DESCRIPTION</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>BodyShop</v>
+        <v>WeldGun01</v>
       </c>
       <c r="B2" t="str">
-        <v>Line1</v>
+        <v>Weld Gun</v>
       </c>
       <c r="C2" t="str">
-        <v>10</v>
+        <v>Body Shop</v>
       </c>
       <c r="D2" t="str">
-        <v>R1</v>
+        <v>OP10</v>
       </c>
       <c r="E2" t="str">
-        <v>KUKA_KR210</v>
+        <v>Servo Gun</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>BodyShop</v>
+        <v>Gripper01</v>
       </c>
       <c r="B3" t="str">
-        <v>Line1</v>
+        <v>Gripper</v>
       </c>
       <c r="C3" t="str">
-        <v>20</v>
+        <v>Body Shop</v>
       </c>
       <c r="D3" t="str">
-        <v>R2</v>
+        <v>OP20</v>
       </c>
       <c r="E3" t="str">
-        <v>KUKA_KR210</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>BodyShop</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Line2</v>
-      </c>
-      <c r="C4" t="str">
-        <v>10</v>
-      </c>
-      <c r="D4" t="str">
-        <v>R3</v>
-      </c>
-      <c r="E4" t="str">
-        <v>ABB_6700</v>
+        <v>Material Handling</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>